<commit_message>
finishe ddata collection for q4
</commit_message>
<xml_diff>
--- a/a2_q4.xlsx
+++ b/a2_q4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CurtisLui/Documents/Documents/SFU /4th Year/SUMMER 2020/CMPT 310/aima-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF1648E-064B-974D-8639-6154C8D28886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED7EB8D-001F-4F4F-90D0-776574AAAD6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22940" windowHeight="21600" xr2:uid="{D9015C34-7CBB-AC41-903C-D4FCB7F2A681}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D9015C34-7CBB-AC41-903C-D4FCB7F2A681}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="I16" sqref="I15:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,8 +651,12 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
         <v>5</v>
@@ -663,11 +667,11 @@
       </c>
       <c r="J5" s="5">
         <f>MAX(B5:F5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="5">
         <f>AVERAGE(B5:F5)</f>
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="L5" s="5">
         <f>MEDIAN(B5:F5)</f>
@@ -687,8 +691,12 @@
       <c r="D6" s="5">
         <v>2.3290660381317099</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="5">
+        <v>3.18053722381591</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3.7076148986816402</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
         <v>6</v>
@@ -699,15 +707,15 @@
       </c>
       <c r="J6" s="5">
         <f t="shared" ref="J6:J9" si="1">MAX(B6:F6)</f>
-        <v>3.2578167915344198</v>
+        <v>3.7076148986816402</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ref="K6:K9" si="2">AVERAGE(B6:F6)</f>
-        <v>2.3940539360046333</v>
+        <v>2.8140627861022898</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" ref="L6:L9" si="3">MEDIAN(B6:F6)</f>
-        <v>2.3290660381317099</v>
+        <v>3.18053722381591</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -723,8 +731,12 @@
       <c r="D7" s="5">
         <v>49</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5">
+        <v>41</v>
+      </c>
+      <c r="F7" s="5">
+        <v>34</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="7" t="s">
         <v>7</v>
@@ -739,11 +751,11 @@
       </c>
       <c r="K7" s="5">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -759,8 +771,12 @@
       <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
         <v>8</v>
@@ -795,8 +811,12 @@
       <c r="D9" s="5">
         <v>49</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="5">
+        <v>51</v>
+      </c>
+      <c r="F9" s="5">
+        <v>54</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
@@ -807,15 +827,15 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="2"/>
-        <v>45.333333333333336</v>
+        <v>48.2</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -895,8 +915,12 @@
       <c r="D13" s="5">
         <v>4</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="5">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="7" t="s">
         <v>5</v>
@@ -911,7 +935,7 @@
       </c>
       <c r="K13" s="5">
         <f>AVERAGE(B13:F13)</f>
-        <v>4.333333333333333</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L13" s="5">
         <f>MEDIAN(B13:F13)</f>
@@ -931,23 +955,27 @@
       <c r="D14" s="5">
         <v>6.1547660827636701</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="5">
+        <v>4.4788880348205504</v>
+      </c>
+      <c r="F14" s="5">
+        <v>8.4062080383300692</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" ref="I14:I17" si="4">MIN(B14:F14)</f>
-        <v>4.87125492095947</v>
+        <v>4.4788880348205504</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" ref="J14:J17" si="5">MAX(B14:F14)</f>
-        <v>6.5982539653777996</v>
+        <v>8.4062080383300692</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ref="K14:K17" si="6">AVERAGE(B14:F14)</f>
-        <v>5.874758323033646</v>
+        <v>6.1018742084503117</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" ref="L14:L17" si="7">MEDIAN(B14:F14)</f>
@@ -967,8 +995,12 @@
       <c r="D15" s="5">
         <v>658</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="5">
+        <v>76</v>
+      </c>
+      <c r="F15" s="5">
+        <v>44</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="7" t="s">
         <v>7</v>
@@ -983,7 +1015,7 @@
       </c>
       <c r="K15" s="5">
         <f t="shared" si="6"/>
-        <v>252.33333333333334</v>
+        <v>175.4</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="7"/>
@@ -1003,8 +1035,12 @@
       <c r="D16" s="5">
         <v>0</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="7" t="s">
         <v>8</v>
@@ -1039,8 +1075,12 @@
       <c r="D17" s="5">
         <v>101</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="5">
+        <v>96</v>
+      </c>
+      <c r="F17" s="5">
+        <v>99</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="7" t="s">
         <v>9</v>
@@ -1055,11 +1095,11 @@
       </c>
       <c r="K17" s="5">
         <f t="shared" si="6"/>
-        <v>94.333333333333329</v>
+        <v>95.6</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="7"/>
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1139,8 +1179,12 @@
       <c r="D21" s="5">
         <v>5</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="5">
+        <v>6</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="7" t="s">
         <v>5</v>
@@ -1151,11 +1195,11 @@
       </c>
       <c r="J21" s="5">
         <f>MAX(B21:F21)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" s="5">
         <f>AVERAGE(B21:F21)</f>
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="L21" s="5">
         <f>MEDIAN(B21:F21)</f>
@@ -1175,8 +1219,12 @@
       <c r="D22" s="5">
         <v>8.2108969688415492</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="5">
+        <v>10.4751739501953</v>
+      </c>
+      <c r="F22">
+        <v>10.411227226257299</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7" t="s">
         <v>6</v>
@@ -1187,15 +1235,15 @@
       </c>
       <c r="J22" s="5">
         <f t="shared" ref="J22:J25" si="9">MAX(B22:F22)</f>
-        <v>9.7781391143798793</v>
+        <v>10.4751739501953</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" ref="K22:K25" si="10">AVERAGE(B22:F22)</f>
-        <v>8.8197444279988559</v>
+        <v>9.4691268920898324</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" ref="L22:L25" si="11">MEDIAN(B22:F22)</f>
-        <v>8.4701972007751394</v>
+        <v>9.7781391143798793</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1211,8 +1259,12 @@
       <c r="D23" s="5">
         <v>46</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="5">
+        <v>68</v>
+      </c>
+      <c r="F23" s="5">
+        <v>164</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="7" t="s">
         <v>7</v>
@@ -1223,11 +1275,11 @@
       </c>
       <c r="J23" s="5">
         <f t="shared" si="9"/>
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="10"/>
-        <v>104</v>
+        <v>108.8</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="11"/>
@@ -1247,8 +1299,12 @@
       <c r="D24" s="5">
         <v>0</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
       <c r="G24" s="5"/>
       <c r="H24" s="7" t="s">
         <v>8</v>
@@ -1283,8 +1339,12 @@
       <c r="D25" s="5">
         <v>130</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="E25" s="5">
+        <v>149</v>
+      </c>
+      <c r="F25" s="5">
+        <v>147</v>
+      </c>
       <c r="G25" s="5"/>
       <c r="H25" s="7" t="s">
         <v>9</v>
@@ -1295,15 +1355,15 @@
       </c>
       <c r="J25" s="5">
         <f t="shared" si="9"/>
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="10"/>
-        <v>136</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="11"/>
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1383,8 +1443,12 @@
       <c r="D29" s="5">
         <v>7</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="E29" s="5">
+        <v>6</v>
+      </c>
+      <c r="F29" s="5">
+        <v>7</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="7" t="s">
         <v>5</v>
@@ -1399,7 +1463,7 @@
       </c>
       <c r="K29" s="5">
         <f>AVERAGE(B29:F29)</f>
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="L29" s="5">
         <f>MEDIAN(B29:F29)</f>
@@ -1419,15 +1483,19 @@
       <c r="D30" s="5">
         <v>18.502534151077199</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="5">
+        <v>12.0614809989929</v>
+      </c>
+      <c r="F30" s="5">
+        <v>18.1896278858184</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" ref="I30:I33" si="12">MIN(B30:F30)</f>
-        <v>13.5351979732513</v>
+        <v>12.0614809989929</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" ref="J30:J33" si="13">MAX(B30:F30)</f>
@@ -1435,11 +1503,11 @@
       </c>
       <c r="K30" s="5">
         <f t="shared" ref="K30:K33" si="14">AVERAGE(B30:F30)</f>
-        <v>18.707410415013566</v>
+        <v>17.274668025970399</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" ref="L30:L33" si="15">MEDIAN(B30:F30)</f>
-        <v>18.502534151077199</v>
+        <v>18.1896278858184</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1455,8 +1523,12 @@
       <c r="D31" s="5">
         <v>48</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="E31" s="5">
+        <v>95</v>
+      </c>
+      <c r="F31" s="5">
+        <v>54</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="7" t="s">
         <v>7</v>
@@ -1471,7 +1543,7 @@
       </c>
       <c r="K31" s="5">
         <f t="shared" si="14"/>
-        <v>74</v>
+        <v>74.2</v>
       </c>
       <c r="L31" s="5">
         <f t="shared" si="15"/>
@@ -1491,8 +1563,12 @@
       <c r="D32" s="5">
         <v>0</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="7" t="s">
         <v>8</v>
@@ -1527,15 +1603,19 @@
       <c r="D33" s="5">
         <v>206</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="E33" s="5">
+        <v>174</v>
+      </c>
+      <c r="F33" s="5">
+        <v>174</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I33" s="5">
         <f t="shared" si="12"/>
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="J33" s="5">
         <f t="shared" si="13"/>
@@ -1543,11 +1623,11 @@
       </c>
       <c r="K33" s="5">
         <f t="shared" si="14"/>
-        <v>195.33333333333334</v>
+        <v>186.8</v>
       </c>
       <c r="L33" s="5">
         <f t="shared" si="15"/>
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -1627,15 +1707,19 @@
       <c r="D37" s="5">
         <v>8</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="5">
+        <v>7</v>
+      </c>
+      <c r="F37" s="5">
+        <v>8</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I37" s="5">
         <f>MIN(B37:F37)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J37" s="5">
         <f>MAX(B37:F37)</f>
@@ -1643,7 +1727,7 @@
       </c>
       <c r="K37" s="5">
         <f>AVERAGE(B37:F37)</f>
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="L37" s="5">
         <f>MEDIAN(B37:F37)</f>
@@ -1663,15 +1747,19 @@
       <c r="D38" s="5">
         <v>24.723447084426802</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="5">
+        <v>17.365117788314802</v>
+      </c>
+      <c r="F38" s="5">
+        <v>24.0473518371582</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I38" s="5">
         <f t="shared" ref="I38:I41" si="16">MIN(B38:F38)</f>
-        <v>24.030010938644399</v>
+        <v>17.365117788314802</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" ref="J38:J41" si="17">MAX(B38:F38)</f>
@@ -1679,11 +1767,11 @@
       </c>
       <c r="K38" s="5">
         <f t="shared" ref="K38:K41" si="18">AVERAGE(B38:F38)</f>
-        <v>24.442921400070134</v>
+        <v>22.94824676513668</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" ref="L38:L41" si="19">MEDIAN(B38:F38)</f>
-        <v>24.575306177139201</v>
+        <v>24.0473518371582</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -1699,8 +1787,12 @@
       <c r="D39" s="5">
         <v>69</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="E39" s="5">
+        <v>125</v>
+      </c>
+      <c r="F39" s="5">
+        <v>41</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="7" t="s">
         <v>7</v>
@@ -1715,7 +1807,7 @@
       </c>
       <c r="K39" s="5">
         <f t="shared" si="18"/>
-        <v>101</v>
+        <v>93.8</v>
       </c>
       <c r="L39" s="5">
         <f t="shared" si="19"/>
@@ -1735,8 +1827,12 @@
       <c r="D40" s="5">
         <v>0</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="7" t="s">
         <v>8</v>
@@ -1771,15 +1867,19 @@
       <c r="D41" s="5">
         <v>230</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="5">
+        <v>221</v>
+      </c>
+      <c r="F41" s="9">
+        <v>226</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I41" s="5">
         <f t="shared" si="16"/>
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J41" s="5">
         <f t="shared" si="17"/>
@@ -1787,11 +1887,11 @@
       </c>
       <c r="K41" s="5">
         <f t="shared" si="18"/>
-        <v>230.66666666666666</v>
+        <v>227.8</v>
       </c>
       <c r="L41" s="5">
         <f t="shared" si="19"/>
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -1871,8 +1971,12 @@
       <c r="D45" s="5">
         <v>10</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="E45" s="5">
+        <v>9</v>
+      </c>
+      <c r="F45" s="5">
+        <v>9</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="7" t="s">
         <v>5</v>
@@ -1907,8 +2011,12 @@
       <c r="D46" s="5">
         <v>33.773796081542898</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="E46" s="5">
+        <v>29.4767711162567</v>
+      </c>
+      <c r="F46" s="5">
+        <v>27.723473310470499</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="7" t="s">
         <v>6</v>
@@ -1923,11 +2031,11 @@
       </c>
       <c r="K46" s="5">
         <f t="shared" ref="K46:K49" si="22">AVERAGE(B46:F46)</f>
-        <v>29.328899701436299</v>
+        <v>29.037388706207217</v>
       </c>
       <c r="L46" s="5">
         <f t="shared" ref="L46:L49" si="23">MEDIAN(B46:F46)</f>
-        <v>31.9349651336669</v>
+        <v>29.4767711162567</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -1943,15 +2051,19 @@
       <c r="D47" s="5">
         <v>89</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="E47" s="5">
+        <v>123</v>
+      </c>
+      <c r="F47" s="5">
+        <v>41</v>
+      </c>
       <c r="G47" s="5"/>
       <c r="H47" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" si="20"/>
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="J47" s="5">
         <f t="shared" si="21"/>
@@ -1959,7 +2071,7 @@
       </c>
       <c r="K47" s="5">
         <f t="shared" si="22"/>
-        <v>109</v>
+        <v>98.2</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="23"/>
@@ -1979,8 +2091,12 @@
       <c r="D48" s="5">
         <v>0</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="E48" s="5">
+        <v>0</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="7" t="s">
         <v>8</v>
@@ -2015,8 +2131,12 @@
       <c r="D49" s="5">
         <v>289</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="5">
+        <v>285</v>
+      </c>
+      <c r="F49" s="5">
+        <v>274</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="7" t="s">
         <v>9</v>
@@ -2031,7 +2151,7 @@
       </c>
       <c r="K49" s="5">
         <f t="shared" si="22"/>
-        <v>273</v>
+        <v>275.60000000000002</v>
       </c>
       <c r="L49" s="5">
         <f t="shared" si="23"/>

</xml_diff>